<commit_message>
added bayesian version, gives very good coverage out of sample
</commit_message>
<xml_diff>
--- a/data/FHM/FHM_latest.xlsx
+++ b/data/FHM/FHM_latest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dfs-srv1.fohm.local\common\Data\covid-19\Do-filer och analys\filer till dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Data\covid-19\Do-filer och analys\filer till dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM 24 Apr 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM 25 Apr 2020" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -165,6 +165,9 @@
     <t>Ålder_70_79</t>
   </si>
   <si>
+    <t>Ålder_80_89</t>
+  </si>
+  <si>
     <t>Ålder_90_plus</t>
   </si>
   <si>
@@ -172,9 +175,6 @@
   </si>
   <si>
     <t>Data uppdateras dagligen kl 11.30 och finns tillgägliga dagligen kl 14.00. Läs mer på https://www.folkhalsomyndigheten.se/smittskydd-beredskap/utbrott/aktuella-utbrott/covid-19/aktuellt-epidemiologiskt-lage/</t>
-  </si>
-  <si>
-    <t>Ålder_80_89</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W82"/>
+  <dimension ref="A1:W83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4705,7 +4705,7 @@
         <v>43923</v>
       </c>
       <c r="B60" s="2">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C60" s="2">
         <v>3</v>
@@ -4741,7 +4741,7 @@
         <v>8</v>
       </c>
       <c r="N60" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O60" s="2">
         <v>34</v>
@@ -4776,7 +4776,7 @@
         <v>43924</v>
       </c>
       <c r="B61" s="2">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C61" s="2">
         <v>1</v>
@@ -4812,7 +4812,7 @@
         <v>24</v>
       </c>
       <c r="N61" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O61" s="2">
         <v>59</v>
@@ -6054,7 +6054,7 @@
         <v>43942</v>
       </c>
       <c r="B79" s="2">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C79" s="2">
         <v>4</v>
@@ -6108,7 +6108,7 @@
         <v>12</v>
       </c>
       <c r="T79" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U79" s="2">
         <v>123</v>
@@ -6196,7 +6196,7 @@
         <v>43944</v>
       </c>
       <c r="B81" s="2">
-        <v>715</v>
+        <v>750</v>
       </c>
       <c r="C81" s="2">
         <v>2</v>
@@ -6205,40 +6205,40 @@
         <v>42</v>
       </c>
       <c r="E81" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F81" s="2">
         <v>13</v>
       </c>
       <c r="G81" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H81" s="2">
         <v>8</v>
       </c>
       <c r="I81" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="J81" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K81" s="2">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L81" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="M81" s="2">
         <v>22</v>
       </c>
       <c r="N81" s="2">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="O81" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P81" s="2">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="Q81" s="2">
         <v>3</v>
@@ -6253,7 +6253,7 @@
         <v>26</v>
       </c>
       <c r="U81" s="2">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="V81" s="2">
         <v>38</v>
@@ -6267,70 +6267,141 @@
         <v>43945</v>
       </c>
       <c r="B82" s="2">
-        <v>294</v>
+        <v>767</v>
       </c>
       <c r="C82" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D82" s="2">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E82" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82" s="2">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="G82" s="2">
+        <v>6</v>
+      </c>
+      <c r="H82" s="2">
+        <v>11</v>
+      </c>
+      <c r="I82" s="2">
+        <v>24</v>
+      </c>
+      <c r="J82" s="2">
+        <v>1</v>
+      </c>
+      <c r="K82" s="2">
+        <v>2</v>
+      </c>
+      <c r="L82" s="2">
+        <v>8</v>
+      </c>
+      <c r="M82" s="2">
+        <v>38</v>
+      </c>
+      <c r="N82" s="2">
+        <v>221</v>
+      </c>
+      <c r="O82" s="2">
+        <v>53</v>
+      </c>
+      <c r="P82" s="2">
+        <v>59</v>
+      </c>
+      <c r="Q82" s="2">
         <v>4</v>
       </c>
-      <c r="H82" s="2">
-        <v>8</v>
-      </c>
-      <c r="I82" s="2">
-        <v>5</v>
-      </c>
-      <c r="J82" s="2">
-        <v>0</v>
-      </c>
-      <c r="K82" s="2">
-        <v>0</v>
-      </c>
-      <c r="L82" s="2">
-        <v>1</v>
-      </c>
-      <c r="M82" s="2">
-        <v>0</v>
-      </c>
-      <c r="N82" s="2">
+      <c r="R82" s="2">
+        <v>12</v>
+      </c>
+      <c r="S82" s="2">
+        <v>16</v>
+      </c>
+      <c r="T82" s="2">
+        <v>36</v>
+      </c>
+      <c r="U82" s="2">
+        <v>147</v>
+      </c>
+      <c r="V82" s="2">
+        <v>41</v>
+      </c>
+      <c r="W82" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23">
+      <c r="A83" s="1">
+        <v>43946</v>
+      </c>
+      <c r="B83" s="2">
         <v>105</v>
       </c>
-      <c r="O82" s="2">
-        <v>30</v>
-      </c>
-      <c r="P82" s="2">
+      <c r="C83" s="2">
+        <v>0</v>
+      </c>
+      <c r="D83" s="2">
+        <v>0</v>
+      </c>
+      <c r="E83" s="2">
+        <v>0</v>
+      </c>
+      <c r="F83" s="2">
+        <v>1</v>
+      </c>
+      <c r="G83" s="2">
+        <v>1</v>
+      </c>
+      <c r="H83" s="2">
+        <v>0</v>
+      </c>
+      <c r="I83" s="2">
+        <v>0</v>
+      </c>
+      <c r="J83" s="2">
+        <v>0</v>
+      </c>
+      <c r="K83" s="2">
+        <v>0</v>
+      </c>
+      <c r="L83" s="2">
+        <v>0</v>
+      </c>
+      <c r="M83" s="2">
+        <v>0</v>
+      </c>
+      <c r="N83" s="2">
+        <v>62</v>
+      </c>
+      <c r="O83" s="2">
+        <v>0</v>
+      </c>
+      <c r="P83" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q83" s="2">
+        <v>0</v>
+      </c>
+      <c r="R83" s="2">
         <v>4</v>
       </c>
-      <c r="Q82" s="2">
-        <v>0</v>
-      </c>
-      <c r="R82" s="2">
-        <v>7</v>
-      </c>
-      <c r="S82" s="2">
-        <v>1</v>
-      </c>
-      <c r="T82" s="2">
-        <v>0</v>
-      </c>
-      <c r="U82" s="2">
-        <v>86</v>
-      </c>
-      <c r="V82" s="2">
-        <v>26</v>
-      </c>
-      <c r="W82" s="2">
-        <v>13</v>
+      <c r="S83" s="2">
+        <v>0</v>
+      </c>
+      <c r="T83" s="2">
+        <v>0</v>
+      </c>
+      <c r="U83" s="2">
+        <v>16</v>
+      </c>
+      <c r="V83" s="2">
+        <v>21</v>
+      </c>
+      <c r="W83" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6342,7 +6413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
@@ -6617,7 +6688,7 @@
         <v>43933</v>
       </c>
       <c r="B34" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -6633,7 +6704,7 @@
         <v>43935</v>
       </c>
       <c r="B36" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -6641,7 +6712,7 @@
         <v>43936</v>
       </c>
       <c r="B37" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -6657,7 +6728,7 @@
         <v>43938</v>
       </c>
       <c r="B39" s="2">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -6665,7 +6736,7 @@
         <v>43939</v>
       </c>
       <c r="B40" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -6673,7 +6744,7 @@
         <v>43940</v>
       </c>
       <c r="B41" s="2">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -6689,7 +6760,7 @@
         <v>43942</v>
       </c>
       <c r="B43" s="2">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -6697,7 +6768,7 @@
         <v>43943</v>
       </c>
       <c r="B44" s="2">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -6705,7 +6776,7 @@
         <v>43944</v>
       </c>
       <c r="B45" s="2">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -6713,7 +6784,7 @@
         <v>43945</v>
       </c>
       <c r="B46" s="2">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -6721,7 +6792,7 @@
         <v>36</v>
       </c>
       <c r="B47" s="2">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -6731,9 +6802,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -6910,7 +6981,7 @@
         <v>43916</v>
       </c>
       <c r="B22" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -6950,7 +7021,7 @@
         <v>43921</v>
       </c>
       <c r="B27" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -6958,7 +7029,7 @@
         <v>43922</v>
       </c>
       <c r="B28" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -7006,7 +7077,7 @@
         <v>43928</v>
       </c>
       <c r="B34" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -7062,7 +7133,7 @@
         <v>43935</v>
       </c>
       <c r="B41" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -7078,7 +7149,7 @@
         <v>43937</v>
       </c>
       <c r="B43" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -7118,7 +7189,7 @@
         <v>43942</v>
       </c>
       <c r="B48" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -7126,7 +7197,7 @@
         <v>43943</v>
       </c>
       <c r="B49" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -7134,7 +7205,7 @@
         <v>43944</v>
       </c>
       <c r="B50" s="2">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -7142,7 +7213,15 @@
         <v>43945</v>
       </c>
       <c r="B51" s="2">
-        <v>9</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1">
+        <v>43946</v>
+      </c>
+      <c r="B52" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7180,10 +7259,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2">
-        <v>35.086399078369141</v>
+        <v>39.472198486328125</v>
       </c>
       <c r="D2" s="2">
         <v>3</v>
@@ -7197,10 +7276,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>612</v>
+        <v>640</v>
       </c>
       <c r="C3" s="2">
-        <v>212.52508544921875</v>
+        <v>222.24845886230469</v>
       </c>
       <c r="D3" s="2">
         <v>35</v>
@@ -7214,10 +7293,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2">
-        <v>36.859565734863281</v>
+        <v>41.885868072509766</v>
       </c>
       <c r="D4" s="2">
         <v>3</v>
@@ -7231,16 +7310,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>475</v>
+        <v>491</v>
       </c>
       <c r="C5" s="2">
-        <v>165.28523254394531</v>
+        <v>170.85273742675781</v>
       </c>
       <c r="D5" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -7248,13 +7327,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C6" s="2">
-        <v>89.262176513671875</v>
+        <v>89.861251831054688</v>
       </c>
       <c r="D6" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2">
         <v>29</v>
@@ -7265,10 +7344,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C7" s="2">
-        <v>199.52603149414063</v>
+        <v>201.81942749023438</v>
       </c>
       <c r="D7" s="2">
         <v>7</v>
@@ -7282,13 +7361,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>636</v>
+        <v>661</v>
       </c>
       <c r="C8" s="2">
-        <v>174.91796875</v>
+        <v>181.79368591308594</v>
       </c>
       <c r="D8" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E8" s="2">
         <v>51</v>
@@ -7299,13 +7378,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C9" s="2">
-        <v>55.816757202148438</v>
+        <v>56.631599426269531</v>
       </c>
       <c r="D9" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2">
         <v>10</v>
@@ -7316,16 +7395,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="C10" s="2">
-        <v>113.16877746582031</v>
+        <v>118.13231658935547</v>
       </c>
       <c r="D10" s="2">
         <v>4</v>
       </c>
       <c r="E10" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7333,10 +7412,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="C11" s="2">
-        <v>87.167572021484375</v>
+        <v>92.365638732910156</v>
       </c>
       <c r="D11" s="2">
         <v>25</v>
@@ -7350,16 +7429,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>606</v>
+        <v>644</v>
       </c>
       <c r="C12" s="2">
-        <v>43.9822998046875</v>
+        <v>46.740264892578125</v>
       </c>
       <c r="D12" s="2">
         <v>56</v>
       </c>
       <c r="E12" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -7367,16 +7446,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>6967</v>
+        <v>7148</v>
       </c>
       <c r="C13" s="2">
-        <v>293.09054565429688</v>
+        <v>300.70492553710938</v>
       </c>
       <c r="D13" s="2">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="E13" s="2">
-        <v>1192</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -7384,10 +7463,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1057</v>
+        <v>1081</v>
       </c>
       <c r="C14" s="2">
-        <v>355.24636840820313</v>
+        <v>363.3125</v>
       </c>
       <c r="D14" s="2">
         <v>83</v>
@@ -7401,16 +7480,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>802</v>
+        <v>862</v>
       </c>
       <c r="C15" s="2">
-        <v>209.0103759765625</v>
+        <v>224.64706420898438</v>
       </c>
       <c r="D15" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E15" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -7418,10 +7497,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C16" s="2">
-        <v>44.615352630615234</v>
+        <v>46.031711578369141</v>
       </c>
       <c r="D16" s="2">
         <v>13</v>
@@ -7435,10 +7514,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="C17" s="2">
-        <v>100.46515655517578</v>
+        <v>103.77719879150391</v>
       </c>
       <c r="D17" s="2">
         <v>24</v>
@@ -7452,16 +7531,16 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="C18" s="2">
-        <v>71.327545166015625</v>
+        <v>77.441337585449219</v>
       </c>
       <c r="D18" s="2">
         <v>16</v>
       </c>
       <c r="E18" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -7469,16 +7548,16 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>625</v>
+        <v>660</v>
       </c>
       <c r="C19" s="2">
-        <v>226.57652282714844</v>
+        <v>239.26480102539063</v>
       </c>
       <c r="D19" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E19" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -7486,16 +7565,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>1886</v>
+        <v>1965</v>
       </c>
       <c r="C20" s="2">
-        <v>109.27751922607422</v>
+        <v>113.85489654541016</v>
       </c>
       <c r="D20" s="2">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="E20" s="2">
-        <v>149</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -7503,16 +7582,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>802</v>
+        <v>838</v>
       </c>
       <c r="C21" s="2">
-        <v>263.11904907226563</v>
+        <v>274.92987060546875</v>
       </c>
       <c r="D21" s="2">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E21" s="2">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -7520,16 +7599,16 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>1305</v>
+        <v>1325</v>
       </c>
       <c r="C22" s="2">
-        <v>280.34674072265625</v>
+        <v>284.64321899414063</v>
       </c>
       <c r="D22" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E22" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -7564,13 +7643,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>7997</v>
+        <v>8237</v>
       </c>
       <c r="C2" s="2">
-        <v>927</v>
+        <v>947</v>
       </c>
       <c r="D2" s="2">
-        <v>1213</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -7578,13 +7657,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>9566</v>
+        <v>9936</v>
       </c>
       <c r="C3" s="2">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="D3" s="2">
-        <v>939</v>
+        <v>956</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7610,9 +7689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -7635,7 +7712,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -7649,7 +7726,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -7663,13 +7740,13 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>1308</v>
+        <v>1370</v>
       </c>
       <c r="C4" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -7677,7 +7754,7 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>1744</v>
+        <v>1813</v>
       </c>
       <c r="C5" s="2">
         <v>57</v>
@@ -7691,10 +7768,10 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>2273</v>
+        <v>2370</v>
       </c>
       <c r="C6" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D6" s="2">
         <v>24</v>
@@ -7705,13 +7782,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>3074</v>
+        <v>3175</v>
       </c>
       <c r="C7" s="2">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="D7" s="2">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -7719,10 +7796,10 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>2336</v>
+        <v>2409</v>
       </c>
       <c r="C8" s="2">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="D8" s="2">
         <v>171</v>
@@ -7733,41 +7810,41 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>2310</v>
+        <v>2372</v>
       </c>
       <c r="C9" s="2">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D9" s="2">
-        <v>507</v>
+        <v>514</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>2763</v>
+        <v>2834</v>
       </c>
       <c r="C10" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2">
-        <v>853</v>
+        <v>869</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>1443</v>
+        <v>1507</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>511</v>
+        <v>525</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -7799,12 +7876,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>